<commit_message>
introduced rules 1st/2nd half of season, cleaning mip
</commit_message>
<xml_diff>
--- a/output/bundesliga_schedule.xlsx
+++ b/output/bundesliga_schedule.xlsx
@@ -70,106 +70,106 @@
     <t>Union Berlin</t>
   </si>
   <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 23</t>
+  </si>
+  <si>
+    <t>Week 24</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 32</t>
+  </si>
+  <si>
+    <t>Week 27</t>
+  </si>
+  <si>
+    <t>Week 29</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 17</t>
+  </si>
+  <si>
+    <t>Week 30</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 21</t>
+  </si>
+  <si>
     <t>Week 1</t>
   </si>
   <si>
-    <t>Week 14</t>
-  </si>
-  <si>
-    <t>Week 27</t>
-  </si>
-  <si>
-    <t>Week 11</t>
+    <t>Week 33</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 16</t>
+  </si>
+  <si>
+    <t>Week 25</t>
+  </si>
+  <si>
+    <t>Week 28</t>
+  </si>
+  <si>
+    <t>Week 26</t>
+  </si>
+  <si>
+    <t>Week 20</t>
+  </si>
+  <si>
+    <t>Week 34</t>
   </si>
   <si>
     <t>Week 13</t>
   </si>
   <si>
-    <t>Week 29</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 33</t>
+    <t>Week 19</t>
+  </si>
+  <si>
+    <t>Week 18</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 15</t>
+  </si>
+  <si>
+    <t>Week 22</t>
   </si>
   <si>
     <t>Week 31</t>
-  </si>
-  <si>
-    <t>Week 20</t>
-  </si>
-  <si>
-    <t>Week 15</t>
-  </si>
-  <si>
-    <t>Week 26</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 25</t>
-  </si>
-  <si>
-    <t>Week 30</t>
-  </si>
-  <si>
-    <t>Week 10</t>
-  </si>
-  <si>
-    <t>Week 18</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 19</t>
-  </si>
-  <si>
-    <t>Week 22</t>
-  </si>
-  <si>
-    <t>Week 16</t>
-  </si>
-  <si>
-    <t>Week 12</t>
-  </si>
-  <si>
-    <t>Week 24</t>
-  </si>
-  <si>
-    <t>Week 34</t>
-  </si>
-  <si>
-    <t>Week 21</t>
-  </si>
-  <si>
-    <t>Week 28</t>
-  </si>
-  <si>
-    <t>Week 32</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 23</t>
-  </si>
-  <si>
-    <t>Week 17</t>
   </si>
 </sst>
 </file>
@@ -597,13 +597,13 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>50</v>
@@ -612,37 +612,37 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
         <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -653,52 +653,52 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
         <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
         <v>48</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -712,49 +712,49 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="s">
         <v>40</v>
       </c>
-      <c r="M4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>50</v>
-      </c>
       <c r="R4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="S4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -765,52 +765,52 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" t="s">
-        <v>41</v>
-      </c>
       <c r="S5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -821,31 +821,31 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="M6" t="s">
         <v>35</v>
@@ -857,16 +857,16 @@
         <v>51</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="Q6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R6" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="S6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -877,52 +877,52 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -933,52 +933,52 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" t="s">
-        <v>38</v>
-      </c>
       <c r="N8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="P8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="R8" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="S8" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -989,52 +989,52 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="M9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" t="s">
         <v>32</v>
-      </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" t="s">
-        <v>31</v>
-      </c>
-      <c r="P9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>43</v>
-      </c>
-      <c r="R9" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1045,52 +1045,52 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" t="s">
-        <v>46</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>24</v>
       </c>
-      <c r="O10" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" t="s">
         <v>35</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1101,52 +1101,52 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="M11" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="N11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="P11" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="Q11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="R11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="S11" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1157,52 +1157,52 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" t="s">
-        <v>38</v>
       </c>
       <c r="K12" t="s">
         <v>39</v>
       </c>
       <c r="M12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>25</v>
+      </c>
+      <c r="R12" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" t="s">
         <v>24</v>
-      </c>
-      <c r="N12" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" t="s">
-        <v>32</v>
-      </c>
-      <c r="P12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" t="s">
-        <v>36</v>
-      </c>
-      <c r="S12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1213,52 +1213,52 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" t="s">
         <v>48</v>
       </c>
-      <c r="J13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" t="s">
-        <v>20</v>
-      </c>
       <c r="O13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="P13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Q13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="R13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="S13" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1269,52 +1269,52 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L14" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="M14" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="O14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="P14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R14" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="S14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1325,52 +1325,52 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" t="s">
-        <v>46</v>
-      </c>
-      <c r="P15" t="s">
-        <v>40</v>
-      </c>
       <c r="Q15" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="R15" t="s">
         <v>19</v>
       </c>
       <c r="S15" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1381,52 +1381,52 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
       </c>
       <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" t="s">
         <v>36</v>
       </c>
-      <c r="I16" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" t="s">
-        <v>34</v>
-      </c>
-      <c r="O16" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>19</v>
-      </c>
       <c r="R16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1437,52 +1437,52 @@
         <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="L17" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="M17" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="N17" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="S17" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1493,52 +1493,52 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" t="s">
         <v>28</v>
       </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="O18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" t="s">
         <v>46</v>
       </c>
-      <c r="I18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="Q18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" t="s">
         <v>42</v>
-      </c>
-      <c r="K18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" t="s">
-        <v>49</v>
-      </c>
-      <c r="O18" t="s">
-        <v>47</v>
-      </c>
-      <c r="P18" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1552,49 +1552,49 @@
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" t="s">
         <v>36</v>
       </c>
-      <c r="H19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" t="s">
-        <v>48</v>
-      </c>
       <c r="K19" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="M19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>27</v>
+      </c>
+      <c r="R19" t="s">
         <v>29</v>
-      </c>
-      <c r="N19" t="s">
-        <v>18</v>
-      </c>
-      <c r="O19" t="s">
-        <v>41</v>
-      </c>
-      <c r="P19" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>